<commit_message>
metrics pipleine working for both cases
</commit_message>
<xml_diff>
--- a/src/metrics/case_1.xlsx
+++ b/src/metrics/case_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -669,217 +669,248 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>mistral_7b_instruct_v3</t>
+          <t>mistral_7b_instruct_v2</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2433</v>
+        <v>2486</v>
       </c>
       <c r="C8" t="n">
-        <v>1501</v>
+        <v>1059</v>
       </c>
       <c r="D8" t="n">
-        <v>1501</v>
+        <v>1295</v>
       </c>
       <c r="E8" t="n">
-        <v>1298</v>
+        <v>1070</v>
       </c>
       <c r="F8" t="n">
-        <v>721</v>
+        <v>155</v>
       </c>
       <c r="G8" t="n">
-        <v>1450</v>
+        <v>107</v>
       </c>
       <c r="H8" t="n">
-        <v>1037</v>
+        <v>66</v>
       </c>
       <c r="I8" t="n">
-        <v>1472</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>mixtral_8x22b_instruct_v01</t>
+          <t>mistral_7b_instruct_v3</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2352</v>
+        <v>2433</v>
       </c>
       <c r="C9" t="n">
-        <v>1862</v>
+        <v>1501</v>
       </c>
       <c r="D9" t="n">
-        <v>1614</v>
+        <v>1501</v>
       </c>
       <c r="E9" t="n">
-        <v>1739</v>
+        <v>1298</v>
       </c>
       <c r="F9" t="n">
-        <v>10</v>
+        <v>721</v>
       </c>
       <c r="G9" t="n">
-        <v>54</v>
+        <v>1450</v>
       </c>
       <c r="H9" t="n">
-        <v>27</v>
+        <v>1037</v>
       </c>
       <c r="I9" t="n">
-        <v>88</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>mixtral_8x7b_instruct_v01</t>
+          <t>mixtral_8x22b_instruct_v01</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2572</v>
+        <v>2352</v>
       </c>
       <c r="C10" t="n">
-        <v>1820</v>
+        <v>1862</v>
       </c>
       <c r="D10" t="n">
-        <v>1834</v>
+        <v>1614</v>
       </c>
       <c r="E10" t="n">
-        <v>1780</v>
+        <v>1739</v>
       </c>
       <c r="F10" t="n">
+        <v>10</v>
+      </c>
+      <c r="G10" t="n">
+        <v>54</v>
+      </c>
+      <c r="H10" t="n">
         <v>27</v>
       </c>
-      <c r="G10" t="n">
-        <v>169</v>
-      </c>
-      <c r="H10" t="n">
-        <v>57</v>
-      </c>
       <c r="I10" t="n">
-        <v>251</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>phi_3_5_moe_instruct</t>
+          <t>mixtral_8x7b_instruct_v01</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1362</v>
+        <v>2572</v>
       </c>
       <c r="C11" t="n">
-        <v>1272</v>
+        <v>1820</v>
       </c>
       <c r="D11" t="n">
-        <v>1059</v>
+        <v>1834</v>
       </c>
       <c r="E11" t="n">
-        <v>1189</v>
+        <v>1780</v>
       </c>
       <c r="F11" t="n">
-        <v>1251</v>
+        <v>27</v>
       </c>
       <c r="G11" t="n">
-        <v>353</v>
+        <v>169</v>
       </c>
       <c r="H11" t="n">
-        <v>425</v>
+        <v>57</v>
       </c>
       <c r="I11" t="n">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>phi_3_small_8k_instruct</t>
+          <t>phi_3_5_moe_instruct</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>966</v>
+        <v>1362</v>
       </c>
       <c r="C12" t="n">
-        <v>831</v>
+        <v>1272</v>
       </c>
       <c r="D12" t="n">
-        <v>591</v>
+        <v>1059</v>
       </c>
       <c r="E12" t="n">
-        <v>735</v>
+        <v>1189</v>
       </c>
       <c r="F12" t="n">
-        <v>524</v>
+        <v>1251</v>
       </c>
       <c r="G12" t="n">
-        <v>531</v>
+        <v>353</v>
       </c>
       <c r="H12" t="n">
-        <v>1177</v>
+        <v>425</v>
       </c>
       <c r="I12" t="n">
-        <v>1000</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>qwen_2_5_14b_instruct</t>
+          <t>phi_3_small_8k_instruct</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1820</v>
+        <v>966</v>
       </c>
       <c r="C13" t="n">
-        <v>813</v>
+        <v>831</v>
       </c>
       <c r="D13" t="n">
-        <v>549</v>
+        <v>591</v>
       </c>
       <c r="E13" t="n">
-        <v>591</v>
+        <v>735</v>
       </c>
       <c r="F13" t="n">
-        <v>1297</v>
+        <v>524</v>
       </c>
       <c r="G13" t="n">
-        <v>1200</v>
+        <v>531</v>
       </c>
       <c r="H13" t="n">
-        <v>1183</v>
+        <v>1177</v>
       </c>
       <c r="I13" t="n">
-        <v>995</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>qwen_2_5_14b_instruct</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1820</v>
+      </c>
+      <c r="C14" t="n">
+        <v>813</v>
+      </c>
+      <c r="D14" t="n">
+        <v>549</v>
+      </c>
+      <c r="E14" t="n">
+        <v>591</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1297</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1200</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1183</v>
+      </c>
+      <c r="I14" t="n">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>qwen_2_5_7b_instruct</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B15" t="n">
         <v>2155</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C15" t="n">
         <v>1145</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D15" t="n">
         <v>920</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E15" t="n">
         <v>1292</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F15" t="n">
         <v>1880</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G15" t="n">
         <v>1619</v>
       </c>
-      <c r="H14" t="n">
+      <c r="H15" t="n">
         <v>1615</v>
       </c>
-      <c r="I14" t="n">
+      <c r="I15" t="n">
         <v>1216</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added details as json data made metrics updation robust to existing files
</commit_message>
<xml_diff>
--- a/src/metrics/case_1.xlsx
+++ b/src/metrics/case_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -576,341 +576,372 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>llama3_8b_instruct</t>
+          <t>llama3_70b_instruct</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1464</v>
+        <v>2296</v>
       </c>
       <c r="C5" t="n">
-        <v>1329</v>
+        <v>1941</v>
       </c>
       <c r="D5" t="n">
-        <v>947</v>
+        <v>1959</v>
       </c>
       <c r="E5" t="n">
-        <v>851</v>
+        <v>1822</v>
       </c>
       <c r="F5" t="n">
-        <v>64</v>
+        <v>272</v>
       </c>
       <c r="G5" t="n">
-        <v>86</v>
+        <v>222</v>
       </c>
       <c r="H5" t="n">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I5" t="n">
-        <v>368</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>llama3_1_8b_instruct</t>
+          <t>llama3_8b_instruct</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1550</v>
+        <v>1464</v>
       </c>
       <c r="C6" t="n">
-        <v>881</v>
+        <v>1329</v>
       </c>
       <c r="D6" t="n">
-        <v>689</v>
+        <v>947</v>
       </c>
       <c r="E6" t="n">
-        <v>829</v>
+        <v>851</v>
       </c>
       <c r="F6" t="n">
-        <v>1118</v>
+        <v>64</v>
       </c>
       <c r="G6" t="n">
-        <v>825</v>
+        <v>86</v>
       </c>
       <c r="H6" t="n">
-        <v>981</v>
+        <v>187</v>
       </c>
       <c r="I6" t="n">
-        <v>992</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>mistral_7b_instruct_v1</t>
+          <t>llama3_1_8b_instruct</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2271</v>
+        <v>1550</v>
       </c>
       <c r="C7" t="n">
-        <v>1181</v>
+        <v>881</v>
       </c>
       <c r="D7" t="n">
-        <v>1425</v>
+        <v>689</v>
       </c>
       <c r="E7" t="n">
-        <v>1209</v>
+        <v>829</v>
       </c>
       <c r="F7" t="n">
-        <v>1753</v>
+        <v>1118</v>
       </c>
       <c r="G7" t="n">
-        <v>2051</v>
+        <v>825</v>
       </c>
       <c r="H7" t="n">
-        <v>1495</v>
+        <v>981</v>
       </c>
       <c r="I7" t="n">
-        <v>1804</v>
+        <v>992</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>mistral_7b_instruct_v2</t>
+          <t>mistral_7b_instruct_v1</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2486</v>
+        <v>2271</v>
       </c>
       <c r="C8" t="n">
-        <v>1059</v>
+        <v>1181</v>
       </c>
       <c r="D8" t="n">
-        <v>1295</v>
+        <v>1425</v>
       </c>
       <c r="E8" t="n">
-        <v>1070</v>
+        <v>1209</v>
       </c>
       <c r="F8" t="n">
-        <v>155</v>
+        <v>1753</v>
       </c>
       <c r="G8" t="n">
-        <v>107</v>
+        <v>2051</v>
       </c>
       <c r="H8" t="n">
-        <v>66</v>
+        <v>1495</v>
       </c>
       <c r="I8" t="n">
-        <v>72</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>mistral_7b_instruct_v3</t>
+          <t>mistral_7b_instruct_v2</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2433</v>
+        <v>2486</v>
       </c>
       <c r="C9" t="n">
-        <v>1501</v>
+        <v>1059</v>
       </c>
       <c r="D9" t="n">
-        <v>1501</v>
+        <v>1295</v>
       </c>
       <c r="E9" t="n">
-        <v>1298</v>
+        <v>1070</v>
       </c>
       <c r="F9" t="n">
-        <v>721</v>
+        <v>155</v>
       </c>
       <c r="G9" t="n">
-        <v>1450</v>
+        <v>107</v>
       </c>
       <c r="H9" t="n">
-        <v>1037</v>
+        <v>66</v>
       </c>
       <c r="I9" t="n">
-        <v>1472</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>mixtral_8x22b_instruct_v01</t>
+          <t>mistral_7b_instruct_v3</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2352</v>
+        <v>2433</v>
       </c>
       <c r="C10" t="n">
-        <v>1862</v>
+        <v>1501</v>
       </c>
       <c r="D10" t="n">
-        <v>1614</v>
+        <v>1501</v>
       </c>
       <c r="E10" t="n">
-        <v>1739</v>
+        <v>1298</v>
       </c>
       <c r="F10" t="n">
-        <v>10</v>
+        <v>721</v>
       </c>
       <c r="G10" t="n">
-        <v>54</v>
+        <v>1450</v>
       </c>
       <c r="H10" t="n">
-        <v>27</v>
+        <v>1037</v>
       </c>
       <c r="I10" t="n">
-        <v>88</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>mixtral_8x7b_instruct_v01</t>
+          <t>mixtral_8x22b_instruct_v01</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2572</v>
+        <v>2352</v>
       </c>
       <c r="C11" t="n">
-        <v>1820</v>
+        <v>1862</v>
       </c>
       <c r="D11" t="n">
-        <v>1834</v>
+        <v>1614</v>
       </c>
       <c r="E11" t="n">
-        <v>1780</v>
+        <v>1739</v>
       </c>
       <c r="F11" t="n">
+        <v>10</v>
+      </c>
+      <c r="G11" t="n">
+        <v>54</v>
+      </c>
+      <c r="H11" t="n">
         <v>27</v>
       </c>
-      <c r="G11" t="n">
-        <v>169</v>
-      </c>
-      <c r="H11" t="n">
-        <v>57</v>
-      </c>
       <c r="I11" t="n">
-        <v>251</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>phi_3_5_moe_instruct</t>
+          <t>mixtral_8x7b_instruct_v01</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1362</v>
+        <v>2572</v>
       </c>
       <c r="C12" t="n">
-        <v>1272</v>
+        <v>1820</v>
       </c>
       <c r="D12" t="n">
-        <v>1059</v>
+        <v>1834</v>
       </c>
       <c r="E12" t="n">
-        <v>1189</v>
+        <v>1780</v>
       </c>
       <c r="F12" t="n">
-        <v>1251</v>
+        <v>27</v>
       </c>
       <c r="G12" t="n">
-        <v>353</v>
+        <v>169</v>
       </c>
       <c r="H12" t="n">
-        <v>425</v>
+        <v>57</v>
       </c>
       <c r="I12" t="n">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>phi_3_small_8k_instruct</t>
+          <t>phi_3_5_moe_instruct</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>966</v>
+        <v>1362</v>
       </c>
       <c r="C13" t="n">
-        <v>831</v>
+        <v>1272</v>
       </c>
       <c r="D13" t="n">
-        <v>591</v>
+        <v>1059</v>
       </c>
       <c r="E13" t="n">
-        <v>735</v>
+        <v>1189</v>
       </c>
       <c r="F13" t="n">
-        <v>524</v>
+        <v>1251</v>
       </c>
       <c r="G13" t="n">
-        <v>531</v>
+        <v>353</v>
       </c>
       <c r="H13" t="n">
-        <v>1177</v>
+        <v>425</v>
       </c>
       <c r="I13" t="n">
-        <v>1000</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>qwen_2_5_14b_instruct</t>
+          <t>phi_3_small_8k_instruct</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1820</v>
+        <v>966</v>
       </c>
       <c r="C14" t="n">
-        <v>813</v>
+        <v>831</v>
       </c>
       <c r="D14" t="n">
-        <v>549</v>
+        <v>591</v>
       </c>
       <c r="E14" t="n">
-        <v>591</v>
+        <v>735</v>
       </c>
       <c r="F14" t="n">
-        <v>1297</v>
+        <v>524</v>
       </c>
       <c r="G14" t="n">
-        <v>1200</v>
+        <v>531</v>
       </c>
       <c r="H14" t="n">
-        <v>1183</v>
+        <v>1177</v>
       </c>
       <c r="I14" t="n">
-        <v>995</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>qwen_2_5_14b_instruct</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1820</v>
+      </c>
+      <c r="C15" t="n">
+        <v>813</v>
+      </c>
+      <c r="D15" t="n">
+        <v>549</v>
+      </c>
+      <c r="E15" t="n">
+        <v>591</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1297</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1200</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1183</v>
+      </c>
+      <c r="I15" t="n">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>qwen_2_5_7b_instruct</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="B16" t="n">
         <v>2155</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C16" t="n">
         <v>1145</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D16" t="n">
         <v>920</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E16" t="n">
         <v>1292</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F16" t="n">
         <v>1880</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G16" t="n">
         <v>1619</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H16" t="n">
         <v>1615</v>
       </c>
-      <c r="I15" t="n">
+      <c r="I16" t="n">
         <v>1216</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated case 1 metrics
</commit_message>
<xml_diff>
--- a/src/metrics/case_1.xlsx
+++ b/src/metrics/case_1.xlsx
@@ -1,37 +1,120 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my_folders\college\research_internships\oracle\multilingual_profanity\src\metrics\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5074C522-8823-4C7B-B9C3-5242E74C646A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>model_name</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>spanish</t>
+  </si>
+  <si>
+    <t>french</t>
+  </si>
+  <si>
+    <t>german</t>
+  </si>
+  <si>
+    <t>hindi</t>
+  </si>
+  <si>
+    <t>marathi</t>
+  </si>
+  <si>
+    <t>bengali</t>
+  </si>
+  <si>
+    <t>gujarati</t>
+  </si>
+  <si>
+    <t>llama3_2_1b_instruct</t>
+  </si>
+  <si>
+    <t>llama3_1_70b_instruct</t>
+  </si>
+  <si>
+    <t>llama3_2_3b_instruct</t>
+  </si>
+  <si>
+    <t>llama3_70b_instruct</t>
+  </si>
+  <si>
+    <t>llama3_8b_instruct</t>
+  </si>
+  <si>
+    <t>llama3_1_8b_instruct</t>
+  </si>
+  <si>
+    <t>mistral_7b_instruct_v1</t>
+  </si>
+  <si>
+    <t>mistral_7b_instruct_v2</t>
+  </si>
+  <si>
+    <t>mistral_7b_instruct_v3</t>
+  </si>
+  <si>
+    <t>mixtral_8x22b_instruct_v01</t>
+  </si>
+  <si>
+    <t>mixtral_8x7b_instruct_v01</t>
+  </si>
+  <si>
+    <t>phi_3_5_moe_instruct</t>
+  </si>
+  <si>
+    <t>phi_3_small_8k_instruct</t>
+  </si>
+  <si>
+    <t>qwen_2_5_14b_instruct</t>
+  </si>
+  <si>
+    <t>qwen_2_5_7b_instruct</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +129,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,528 +453,479 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>model_name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>english</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>spanish</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>french</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>german</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>hindi</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>marathi</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>bengali</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>gujarati</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>llama3_2_1b_instruct</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
         <v>958</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>161</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>205</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>408</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>336</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>826</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>1073</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2">
         <v>958</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>llama3_1_70b_instruct</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
         <v>1846</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>1247</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>1521</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>1386</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>1380</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>809</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3">
         <v>1390</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3">
         <v>728</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>llama3_2_3b_instruct</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
         <v>1529</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>675</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>671</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>538</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>776</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>610</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4">
         <v>839</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4">
         <v>631</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>llama3_70b_instruct</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
         <v>2296</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>1941</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>1959</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>1822</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>272</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>222</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5">
         <v>185</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I5">
         <v>1</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>llama3_8b_instruct</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
         <v>1464</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>1329</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>947</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>851</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>64</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>86</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6">
         <v>187</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6">
         <v>368</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>llama3_1_8b_instruct</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
         <v>1550</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>881</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>689</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>829</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>1118</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>825</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7">
         <v>981</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7">
         <v>992</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>mistral_7b_instruct_v1</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
         <v>2271</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>1181</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>1425</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>1209</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8">
         <v>1753</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8">
         <v>2051</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8">
         <v>1495</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8">
         <v>1804</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>mistral_7b_instruct_v2</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
         <v>2486</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>1059</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>1295</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>1070</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>155</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9">
         <v>107</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H9">
         <v>66</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I9">
         <v>72</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>mistral_7b_instruct_v3</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
         <v>2433</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>1501</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>1501</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>1298</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10">
         <v>721</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10">
         <v>1450</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H10">
         <v>1037</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I10">
         <v>1472</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>mixtral_8x22b_instruct_v01</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
         <v>2352</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>1862</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>1614</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>1739</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11">
         <v>10</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11">
         <v>54</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H11">
         <v>27</v>
       </c>
-      <c r="I11" t="n">
+      <c r="I11">
         <v>88</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>mixtral_8x7b_instruct_v01</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
         <v>2572</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12">
         <v>1820</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12">
         <v>1834</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12">
         <v>1780</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12">
         <v>27</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G12">
         <v>169</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H12">
         <v>57</v>
       </c>
-      <c r="I12" t="n">
+      <c r="I12">
         <v>251</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>phi_3_5_moe_instruct</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
         <v>1362</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13">
         <v>1272</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13">
         <v>1059</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13">
         <v>1189</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13">
         <v>1251</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G13">
         <v>353</v>
       </c>
-      <c r="H13" t="n">
+      <c r="H13">
         <v>425</v>
       </c>
-      <c r="I13" t="n">
+      <c r="I13">
         <v>247</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>phi_3_small_8k_instruct</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
         <v>966</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14">
         <v>831</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14">
         <v>591</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14">
         <v>735</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F14">
         <v>524</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G14">
         <v>531</v>
       </c>
-      <c r="H14" t="n">
+      <c r="H14">
         <v>1177</v>
       </c>
-      <c r="I14" t="n">
+      <c r="I14">
         <v>1000</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>qwen_2_5_14b_instruct</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
         <v>1820</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15">
         <v>813</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15">
         <v>549</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15">
         <v>591</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F15">
         <v>1297</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G15">
         <v>1200</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H15">
         <v>1183</v>
       </c>
-      <c r="I15" t="n">
+      <c r="I15">
         <v>995</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>qwen_2_5_7b_instruct</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
         <v>2155</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16">
         <v>1145</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16">
         <v>920</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16">
         <v>1292</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F16">
         <v>1880</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G16">
         <v>1619</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H16">
         <v>1615</v>
       </c>
-      <c r="I16" t="n">
+      <c r="I16">
         <v>1216</v>
       </c>
     </row>

</xml_diff>